<commit_message>
UPDATED test plan for coverage
</commit_message>
<xml_diff>
--- a/docs/DMA_Test_Plan.xlsx
+++ b/docs/DMA_Test_Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MProjects\DMA RAL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3999C71F-5651-4B06-9F44-DA6CA0759783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E7E365-0D27-4428-85B8-4B1C78EF2469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
   <si>
     <t>Feature ID</t>
   </si>
@@ -99,15 +99,9 @@
     <t>C</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>REGISTER COVERPOINTS</t>
   </si>
   <si>
-    <t>REGISTER CROSS COVERAGE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Register </t>
   </si>
   <si>
@@ -339,12 +333,6 @@
     <t>config_cp</t>
   </si>
   <si>
-    <t>ctrlxio</t>
-  </si>
-  <si>
-    <t>ctrlxmem</t>
-  </si>
-  <si>
     <t>Checks the fields of INTR reg</t>
   </si>
   <si>
@@ -373,16 +361,13 @@
   </si>
   <si>
     <t>Checks the fields of DESCRIPTOR_ADDR reg</t>
-  </si>
-  <si>
-    <t>Check the addressing from mem to io and io to mem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,12 +423,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <charset val="1"/>
     </font>
     <font>
@@ -830,7 +809,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -910,13 +889,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -949,7 +922,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -958,31 +931,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1513,14 +1486,14 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>23</v>
+      <c r="D1" s="30" t="s">
+        <v>21</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1539,25 +1512,25 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1">
-      <c r="A2" s="33">
+      <c r="A2" s="31">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="33" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="6"/>
@@ -1570,22 +1543,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="34" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>30</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="9" t="s">
@@ -1597,22 +1570,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="38" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>32</v>
+      <c r="G4" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="9" t="s">
@@ -1624,22 +1597,22 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>26</v>
+        <v>43</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>32</v>
+        <v>60</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="9" t="s">
@@ -1647,26 +1620,26 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.4">
-      <c r="A6" s="33">
+      <c r="A6" s="31">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>37</v>
+        <v>72</v>
+      </c>
+      <c r="C6" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>35</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>32</v>
+        <v>61</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="9" t="s">
@@ -1678,22 +1651,22 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="41" t="s">
-        <v>44</v>
+        <v>72</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>42</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="36" t="s">
-        <v>32</v>
+        <v>62</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="9" t="s">
@@ -1705,22 +1678,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>38</v>
+        <v>72</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="36" t="s">
-        <v>32</v>
+        <v>62</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="9" t="s">
@@ -1732,22 +1705,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="41" t="s">
-        <v>39</v>
+        <v>72</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>37</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="36" t="s">
-        <v>32</v>
+        <v>63</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="9" t="s">
@@ -1755,26 +1728,26 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.4">
-      <c r="A10" s="33">
+      <c r="A10" s="31">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>40</v>
+        <v>72</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="36" t="s">
-        <v>32</v>
+        <v>64</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="9" t="s">
@@ -1786,22 +1759,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>41</v>
+        <v>72</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>39</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="9" t="s">
@@ -1813,22 +1786,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>42</v>
+        <v>72</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>40</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>32</v>
+        <v>65</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>30</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="9" t="s">
@@ -1840,25 +1813,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>43</v>
+        <v>72</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>41</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>30</v>
       </c>
       <c r="H13" s="11"/>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="36" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1906,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="1"/>
@@ -1949,26 +1922,26 @@
       <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
+      <c r="B2" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickTop="1">
       <c r="A3" s="25">
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E3" s="13">
         <v>2</v>
@@ -1982,18 +1955,18 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>81</v>
+        <v>70</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>79</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="30">
+        <v>86</v>
+      </c>
+      <c r="E4" s="28">
         <v>2</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="F4" s="43" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2002,13 +1975,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E5" s="1">
         <v>2</v>
@@ -2022,13 +1995,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1">
         <v>64</v>
@@ -2042,13 +2015,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
@@ -2062,13 +2035,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E8" s="11">
         <v>5</v>
@@ -2081,23 +2054,23 @@
       <c r="A9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
+      <c r="B9" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickTop="1">
       <c r="A10" s="13">
         <v>7</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="13">
@@ -2108,44 +2081,44 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1">
-      <c r="A11" s="48">
+      <c r="A11" s="44">
         <v>8</v>
       </c>
-      <c r="B11" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="48">
+      <c r="B11" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="E11" s="44">
         <v>320</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="46" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
+      <c r="B12" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickTop="1">
       <c r="A13" s="13">
         <v>1</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="13"/>
@@ -2158,10 +2131,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
@@ -2174,10 +2147,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
@@ -2190,10 +2163,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
@@ -2206,10 +2179,10 @@
         <v>5</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
@@ -2222,10 +2195,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
@@ -2238,10 +2211,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
@@ -2254,10 +2227,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="1"/>
@@ -2270,10 +2243,10 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
@@ -2286,10 +2259,10 @@
         <v>10</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="11"/>
@@ -2297,59 +2270,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16.8" thickTop="1" thickBot="1">
-      <c r="A23" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" thickTop="1">
-      <c r="A24" s="27">
-        <v>11</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" thickBot="1">
-      <c r="A25" s="11">
-        <v>12</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" thickTop="1"/>
+    <row r="23" spans="1:6" ht="15" thickTop="1"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B23:F23"/>
   </mergeCells>
-  <conditionalFormatting sqref="F3:F8 F10:F11 F13:F22 F24:F25">
+  <conditionalFormatting sqref="F3:F8 F10:F11 F13:F22">
     <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="IGNORED">
       <formula>NOT(ISERROR(SEARCH("IGNORED",F3)))</formula>
     </cfRule>
@@ -2376,7 +2304,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24:F25 F13:F22 F10:F11 F3:F8" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F22 F10:F11 F3:F8" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"NOT STARTED,INCOMPLETE,COVERED,IGNORED"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2401,7 +2329,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F3:F8 F10:F11 F13:F22 F24:F25</xm:sqref>
+          <xm:sqref>F3:F8 F10:F11 F13:F22</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
UPDATED the test plan to check
</commit_message>
<xml_diff>
--- a/docs/DMA_Test_Plan.xlsx
+++ b/docs/DMA_Test_Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MProjects\DMA RAL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E7E365-0D27-4428-85B8-4B1C78EF2469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1B84B5-E99A-4857-817E-A377FC941C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="1" state="hidden" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="113">
   <si>
     <t>Feature ID</t>
   </si>
@@ -361,6 +361,21 @@
   </si>
   <si>
     <t>Checks the fields of DESCRIPTOR_ADDR reg</t>
+  </si>
+  <si>
+    <t>32'h400,'h404,'h408,'h40C,'h412,'h416,'h420,'h424</t>
+  </si>
+  <si>
+    <t>8(others are not included)</t>
+  </si>
+  <si>
+    <t>extra_info_test</t>
+  </si>
+  <si>
+    <t>EXTRA_INFO</t>
+  </si>
+  <si>
+    <t>Test the info field</t>
   </si>
 </sst>
 </file>
@@ -809,7 +824,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -952,6 +967,9 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -960,6 +978,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1462,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="1"/>
@@ -1701,23 +1725,23 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.4">
-      <c r="A9" s="1">
+      <c r="A9" s="31">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>37</v>
+        <v>110</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>111</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="G9" s="34" t="s">
         <v>30</v>
@@ -1728,23 +1752,23 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.4">
-      <c r="A10" s="31">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="G10" s="34" t="s">
         <v>30</v>
@@ -1755,23 +1779,23 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.4">
-      <c r="A11" s="1">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C11" s="41" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="G11" s="34" t="s">
         <v>30</v>
@@ -1781,63 +1805,90 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.4">
-      <c r="A12" s="10">
+    <row r="12" spans="1:9" ht="15" thickBot="1">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" s="34" t="s">
+      <c r="C12" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="9" t="s">
+      <c r="H12" s="11"/>
+      <c r="I12" s="36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1">
-      <c r="A13" s="11">
-        <v>12</v>
-      </c>
-      <c r="B13" s="17" t="s">
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" thickTop="1"/>
+    <row r="15" spans="1:9" ht="14.4">
+      <c r="A15" s="31">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" s="35" t="s">
+      <c r="C15" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="11"/>
-      <c r="I13" s="36" t="s">
+      <c r="H15" s="1"/>
+      <c r="I15" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickTop="1"/>
+    <row r="16" spans="1:9" ht="14.4">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G12 G15:G16">
     <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="LOW">
       <formula>NOT(ISERROR(SEARCH("LOW",G2)))</formula>
     </cfRule>
@@ -1848,7 +1899,7 @@
       <formula>NOT(ISERROR(SEARCH("MED",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I12 I15:I16">
     <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="FAILED">
       <formula>NOT(ISERROR(SEARCH("FAILED",I2)))</formula>
     </cfRule>
@@ -1863,11 +1914,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I13" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I15:I16 I2:I8 I9:I12" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"NOT COMPLETED,FAILED,PASSED"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G15:G16 G2:G8 G9:G12" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"HIGH,MED,LOW"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1881,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" customHeight="1"/>
@@ -1890,8 +1941,8 @@
     <col min="1" max="1" width="7.88671875" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="62.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.44140625" style="3" customWidth="1"/>
     <col min="7" max="9" width="8.88671875" style="3"/>
     <col min="10" max="10" width="38.109375" style="3" customWidth="1"/>
@@ -1922,13 +1973,13 @@
       <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickTop="1">
       <c r="A3" s="25">
@@ -2000,11 +2051,11 @@
       <c r="C6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>87</v>
+      <c r="D6" s="48" t="s">
+        <v>108</v>
       </c>
       <c r="E6" s="1">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="F6" s="20" t="s">
         <v>13</v>
@@ -2024,7 +2075,7 @@
         <v>87</v>
       </c>
       <c r="E7" s="1">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>13</v>
@@ -2044,7 +2095,7 @@
         <v>87</v>
       </c>
       <c r="E8" s="11">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>13</v>
@@ -2054,13 +2105,13 @@
       <c r="A9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickTop="1">
       <c r="A10" s="13">
@@ -2073,8 +2124,8 @@
         <v>84</v>
       </c>
       <c r="D10" s="18"/>
-      <c r="E10" s="13">
-        <v>320</v>
+      <c r="E10" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="F10" s="19" t="s">
         <v>13</v>
@@ -2091,8 +2142,8 @@
         <v>85</v>
       </c>
       <c r="D11" s="45"/>
-      <c r="E11" s="44">
-        <v>320</v>
+      <c r="E11" s="44" t="s">
+        <v>109</v>
       </c>
       <c r="F11" s="46" t="s">
         <v>13</v>
@@ -2102,13 +2153,13 @@
       <c r="A12" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickTop="1">
       <c r="A13" s="13">

</xml_diff>